<commit_message>
Final - After Session
</commit_message>
<xml_diff>
--- a/psconfeu2019/Community/psconfeu2019.xlsx
+++ b/psconfeu2019/Community/psconfeu2019.xlsx
@@ -1183,6 +1183,104 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>PowerShell Conference EU 2019 - Speakers</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Series 1</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'SpeakerCountryChart'!Name</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SpeakerCountryChart'!Count</c:f>
+            </c:numRef>
+          </c:val>
+        </ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+          </c:separator>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:chart>
     <c:title>
@@ -1312,6 +1410,36 @@
     </graphicFrame>
     <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="ChartF220"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1324,6 +1452,19 @@
     <tableColumn id="3" name="Ends"/>
     <tableColumn id="4" name="Track"/>
     <tableColumn id="5" name="Speaker"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A2:D49" headerRowCount="1">
+  <autoFilter ref="A2:D49"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="FirstName"/>
+    <tableColumn id="2" name="LastName"/>
+    <tableColumn id="3" name="Twitter"/>
+    <tableColumn id="4" name="Country"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1381,6 +1522,59 @@
 </table>
 </file>
 
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:E122" headerRowCount="1">
+  <autoFilter ref="A2:E122"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Starts"/>
+    <tableColumn id="3" name="Ends"/>
+    <tableColumn id="4" name="Track"/>
+    <tableColumn id="5" name="Speaker"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:D29" headerRowCount="1">
+  <autoFilter ref="A2:D29"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Starts"/>
+    <tableColumn id="3" name="Ends"/>
+    <tableColumn id="4" name="Speaker"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A2:D35" headerRowCount="1">
+  <autoFilter ref="A2:D35"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Starts"/>
+    <tableColumn id="3" name="Ends"/>
+    <tableColumn id="4" name="Speaker"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A2:D36" headerRowCount="1">
+  <autoFilter ref="A2:D36"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Starts"/>
+    <tableColumn id="3" name="Ends"/>
+    <tableColumn id="4" name="Speaker"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E122"/>
@@ -3455,6 +3649,7 @@
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3868,6 +4063,7 @@
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4365,6 +4561,7 @@
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4876,6 +5073,7 @@
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5569,6 +5767,7 @@
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>